<commit_message>
Add Victoria, Michigan and Superior to test
</commit_message>
<xml_diff>
--- a/data/Sample.xlsx
+++ b/data/Sample.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olden/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HydroATLAS_sampleR\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{76C0A975-F633-1D4A-83CC-7D7F17C7546E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8780" yWindow="4100" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{3BAE83D8-4486-DF42-A8E5-F60A11D28131}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11100" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="River sample" sheetId="1" r:id="rId1"/>
     <sheet name="Lake sample" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="589">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="597">
   <si>
     <t>FW_ID</t>
   </si>
@@ -1804,13 +1803,37 @@
   </si>
   <si>
     <t>Clairvaux_Jura_region</t>
+  </si>
+  <si>
+    <t>Superior</t>
+  </si>
+  <si>
+    <t>FWB_999</t>
+  </si>
+  <si>
+    <t>FWB_997</t>
+  </si>
+  <si>
+    <t>Michigan</t>
+  </si>
+  <si>
+    <t>FWB_998</t>
+  </si>
+  <si>
+    <t>Victoria</t>
+  </si>
+  <si>
+    <t>UGA</t>
+  </si>
+  <si>
+    <t>Uganda</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1913,7 +1936,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Style0" xfId="1" xr:uid="{84FC2E82-BEFB-8F49-A5CF-A5ECA179E35F}"/>
+    <cellStyle name="Style0" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2244,19 +2267,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2935A85C-F164-CD4D-B056-925BB5DA8BBE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:KR11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="9" width="10.83203125" style="3"/>
+    <col min="1" max="9" width="10.77734375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:304" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:304" ht="16.5" thickBot="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3170,7 +3193,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="2" spans="1:304" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:304">
       <c r="A2" s="3" t="s">
         <v>304</v>
       </c>
@@ -4084,7 +4107,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="3" spans="1:304" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:304">
       <c r="A3" s="3" t="s">
         <v>311</v>
       </c>
@@ -4998,7 +5021,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="4" spans="1:304" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:304">
       <c r="A4" s="3" t="s">
         <v>313</v>
       </c>
@@ -5912,7 +5935,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="5" spans="1:304" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:304">
       <c r="A5" s="3" t="s">
         <v>317</v>
       </c>
@@ -6826,7 +6849,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="6" spans="1:304" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:304">
       <c r="A6" s="3" t="s">
         <v>319</v>
       </c>
@@ -7740,7 +7763,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="7" spans="1:304" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:304">
       <c r="A7" s="3" t="s">
         <v>324</v>
       </c>
@@ -8654,7 +8677,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="8" spans="1:304" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:304">
       <c r="A8" s="3" t="s">
         <v>326</v>
       </c>
@@ -9568,7 +9591,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="9" spans="1:304" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:304">
       <c r="A9" s="3" t="s">
         <v>328</v>
       </c>
@@ -10482,7 +10505,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="10" spans="1:304" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:304">
       <c r="A10" s="3" t="s">
         <v>330</v>
       </c>
@@ -11396,7 +11419,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="11" spans="1:304" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:304">
       <c r="A11" s="3" t="s">
         <v>332</v>
       </c>
@@ -12316,19 +12339,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D4CAC90-B3B3-C541-BB9A-4064DCF92FE4}">
-  <dimension ref="A1:LD11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:LD14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I1048576"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="9" width="10.83203125" style="3"/>
+    <col min="1" max="9" width="10.77734375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:316" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:316" ht="15.75">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -13273,7 +13296,7 @@
       </c>
       <c r="LC1" s="5"/>
     </row>
-    <row r="2" spans="1:316" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:316" ht="15.75">
       <c r="A2" s="8" t="s">
         <v>549</v>
       </c>
@@ -14219,7 +14242,7 @@
       <c r="LC2" s="5"/>
       <c r="LD2" s="5"/>
     </row>
-    <row r="3" spans="1:316" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:316" ht="15.75">
       <c r="A3" s="8" t="s">
         <v>558</v>
       </c>
@@ -15165,7 +15188,7 @@
       <c r="LC3" s="5"/>
       <c r="LD3" s="5"/>
     </row>
-    <row r="4" spans="1:316" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:316" ht="15.75">
       <c r="A4" s="8" t="s">
         <v>561</v>
       </c>
@@ -16109,7 +16132,7 @@
       <c r="LC4" s="5"/>
       <c r="LD4" s="5"/>
     </row>
-    <row r="5" spans="1:316" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:316" ht="15.75">
       <c r="A5" s="8" t="s">
         <v>568</v>
       </c>
@@ -17053,7 +17076,7 @@
       <c r="LC5" s="5"/>
       <c r="LD5" s="5"/>
     </row>
-    <row r="6" spans="1:316" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:316" ht="15.75">
       <c r="A6" s="8" t="s">
         <v>570</v>
       </c>
@@ -17999,7 +18022,7 @@
       <c r="LC6" s="5"/>
       <c r="LD6" s="5"/>
     </row>
-    <row r="7" spans="1:316" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:316" ht="15.75">
       <c r="A7" s="8" t="s">
         <v>575</v>
       </c>
@@ -18945,7 +18968,7 @@
       <c r="LC7" s="5"/>
       <c r="LD7" s="5"/>
     </row>
-    <row r="8" spans="1:316" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:316" ht="15.75">
       <c r="A8" s="8" t="s">
         <v>580</v>
       </c>
@@ -19891,7 +19914,7 @@
       <c r="LC8" s="5"/>
       <c r="LD8" s="5"/>
     </row>
-    <row r="9" spans="1:316" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:316" ht="15.75">
       <c r="A9" s="8" t="s">
         <v>581</v>
       </c>
@@ -20835,7 +20858,7 @@
       <c r="LC9" s="5"/>
       <c r="LD9" s="5"/>
     </row>
-    <row r="10" spans="1:316" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:316" ht="15.75">
       <c r="A10" s="8" t="s">
         <v>585</v>
       </c>
@@ -21779,7 +21802,7 @@
       <c r="LC10" s="5"/>
       <c r="LD10" s="5"/>
     </row>
-    <row r="11" spans="1:316" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:316" ht="15.75">
       <c r="A11" s="8" t="s">
         <v>587</v>
       </c>
@@ -22722,6 +22745,93 @@
       </c>
       <c r="LC11" s="5"/>
       <c r="LD11" s="5"/>
+    </row>
+    <row r="12" spans="1:316" ht="15.75">
+      <c r="A12" s="8" t="s">
+        <v>591</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>562</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>321</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>589</v>
+      </c>
+      <c r="H12" s="8">
+        <v>46.468592999999998</v>
+      </c>
+      <c r="I12" s="8">
+        <v>-84.460547000000005</v>
+      </c>
+    </row>
+    <row r="13" spans="1:316" ht="15.75">
+      <c r="A13" s="8" t="s">
+        <v>593</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>562</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>321</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>592</v>
+      </c>
+      <c r="H13" s="8">
+        <v>45.822915999999999</v>
+      </c>
+      <c r="I13" s="8">
+        <v>-84.753910000000005</v>
+      </c>
+    </row>
+    <row r="14" spans="1:316" ht="15.75">
+      <c r="A14" s="8" t="s">
+        <v>590</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>562</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>595</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>596</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>594</v>
+      </c>
+      <c r="H14" s="8">
+        <v>0.43099900000000002</v>
+      </c>
+      <c r="I14" s="8">
+        <v>33.193790999999997</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>